<commit_message>
Add support to read logfiles from campaign, rename spectrum_analyzer_test.
</commit_message>
<xml_diff>
--- a/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
+++ b/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matro\Documents\AIUC\Scripts\RFLabTests\rf_measures_powervoltage_curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0C4814-1CE4-44C8-B599-A72805732F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B542FC56-D2D0-4ED0-825E-FCD34D7F4398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ajuste 14-15 dec" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
   <si>
     <t>Voltage Attenuation</t>
   </si>
@@ -153,6 +153,12 @@
   <si>
     <t>ADC old scaled</t>
   </si>
+  <si>
+    <t>ADC measured (in volts)</t>
+  </si>
+  <si>
+    <t>ADC measured (in Volts)</t>
+  </si>
 </sst>
 </file>
 
@@ -221,6 +227,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Power Measured (dBm) vs Voltage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> attenuation input (V)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -261,7 +296,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ajuste 14-15 dec'!$D$2</c:f>
+              <c:f>'Ajuste 14-15 dec'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -404,7 +439,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ajuste 14-15 dec'!$D$3:$D$18</c:f>
+              <c:f>'Ajuste 14-15 dec'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -668,6 +703,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Power Measured (dBm) vs ADC measured</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CL" baseline="0"/>
+              <a:t> (V)</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -708,7 +773,454 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ajuste 8-13 dec'!$D$2</c:f>
+              <c:f>'Ajuste 14-15 dec'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Measured (dBm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.2657130358705162"/>
+                  <c:y val="-1.4399241761446485E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ajuste 14-15 dec'!$D$3:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.20645161290322581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30967741935483867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46129032258064512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61935483870967734</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82258064516129037</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0419354838709676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2774193548387096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4193548387096775</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5290322580645159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7806451612903225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0161290322580645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2193548387096773</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3838709677419354</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5290322580645159</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6451612903225805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7483870967741932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ajuste 14-15 dec'!$E$3:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-75.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-73.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-71.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-70.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-67.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-66.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-65.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-65.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-64.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-63.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-62.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-61.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-61.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-60.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-59.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89C7-4B3D-99F8-EAF3A00771F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1307452063"/>
+        <c:axId val="1307452479"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1307452063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307452479"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1307452479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1307452063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ajuste 8-13 dec'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,7 +1363,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ajuste 8-13 dec'!$D$3:$D$18</c:f>
+              <c:f>'Ajuste 8-13 dec'!$E$3:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1100,7 +1612,430 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ajuste 8-13 dec'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power Measured (dBm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.2197425634295713"/>
+                  <c:y val="-4.6583916593759114E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ajuste 8-13 dec'!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.51935483870967736</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70645161290322578</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95161290322580649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2290322580645161</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5580645161290321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9096774193548387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2161290322580642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3548387096774195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4709677419354836</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6516129032258062</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7870967741935484</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8516129032258064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ajuste 8-13 dec'!$E$3:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-76.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-74.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-69.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-68.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-66.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-65.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-64.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-63.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-63.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BDF-4488-8AB2-6AC04ABE7767}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1028650015"/>
+        <c:axId val="1028652927"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1028650015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028652927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1028652927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028650015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2144,7 +3079,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -3126,7 +4061,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -4041,6 +4976,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6106,6 +7121,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6631,7 +8678,7 @@
       <xdr:rowOff>141922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>168592</xdr:rowOff>
@@ -6659,6 +8706,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B2E1E-FB06-45A9-8475-738F29A64A1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6672,7 +8755,7 @@
       <xdr:rowOff>141922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>168592</xdr:rowOff>
@@ -6697,6 +8780,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32810FB2-7BF1-41FB-9432-82EC6F0EF1C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7083,19 +9202,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -7103,10 +9222,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0.2</v>
       </c>
@@ -7114,16 +9236,20 @@
         <v>64</v>
       </c>
       <c r="D3">
+        <f>3.3*C3/1023</f>
+        <v>0.20645161290322581</v>
+      </c>
+      <c r="E3">
         <v>-75.900000000000006</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -7131,16 +9257,20 @@
         <v>96</v>
       </c>
       <c r="D4">
+        <f t="shared" ref="D4:D18" si="0">3.3*C4/1023</f>
+        <v>0.30967741935483867</v>
+      </c>
+      <c r="E4">
         <v>-73.8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0.6</v>
       </c>
@@ -7148,16 +9278,20 @@
         <v>143</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.46129032258064512</v>
+      </c>
+      <c r="E5">
         <v>-71.8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.8</v>
       </c>
@@ -7165,16 +9299,20 @@
         <v>192</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.61935483870967734</v>
+      </c>
+      <c r="E6">
         <v>-70.2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -7182,13 +9320,17 @@
         <v>255</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.82258064516129037</v>
+      </c>
+      <c r="E7">
         <v>-68.599999999999994</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.2</v>
       </c>
@@ -7196,13 +9338,17 @@
         <v>323</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.0419354838709676</v>
+      </c>
+      <c r="E8">
         <v>-67.3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -7210,13 +9356,17 @@
         <v>396</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.2774193548387096</v>
+      </c>
+      <c r="E9">
         <v>-66.099999999999994</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.5</v>
       </c>
@@ -7224,16 +9374,20 @@
         <v>440</v>
       </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.4193548387096775</v>
+      </c>
+      <c r="E10">
         <v>-65.5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1.6</v>
       </c>
@@ -7241,16 +9395,20 @@
         <v>474</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.5290322580645159</v>
+      </c>
+      <c r="E11">
         <v>-65.099999999999994</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1.8</v>
       </c>
@@ -7258,16 +9416,20 @@
         <v>552</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.7806451612903225</v>
+      </c>
+      <c r="E12">
         <v>-64.099999999999994</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2</v>
       </c>
@@ -7275,16 +9437,20 @@
         <v>625</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="E13">
         <v>-63.2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2.2000000000000002</v>
       </c>
@@ -7292,16 +9458,20 @@
         <v>688</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2.2193548387096773</v>
+      </c>
+      <c r="E14">
         <v>-62.3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.4</v>
       </c>
@@ -7309,16 +9479,20 @@
         <v>739</v>
       </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>2.3838709677419354</v>
+      </c>
+      <c r="E15">
         <v>-61.6</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2.6</v>
       </c>
@@ -7326,13 +9500,17 @@
         <v>784</v>
       </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>2.5290322580645159</v>
+      </c>
+      <c r="E16">
         <v>-61.1</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2.8</v>
       </c>
@@ -7340,16 +9518,20 @@
         <v>820</v>
       </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.6451612903225805</v>
+      </c>
+      <c r="E17">
         <v>-60.4</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3</v>
       </c>
@@ -7357,12 +9539,16 @@
         <v>852</v>
       </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.7483870967741932</v>
+      </c>
+      <c r="E18">
         <v>-59.8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7374,19 +9560,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501F32F7-C9D6-47EE-A900-3F721E2AB069}">
-  <dimension ref="B2:F18"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="17.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -7394,10 +9580,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0.2</v>
       </c>
@@ -7405,16 +9594,20 @@
         <v>161</v>
       </c>
       <c r="D3">
+        <f>3.3*C3/1023</f>
+        <v>0.51935483870967736</v>
+      </c>
+      <c r="E3">
         <v>-76.900000000000006</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -7422,16 +9615,20 @@
         <v>219</v>
       </c>
       <c r="D4">
+        <f t="shared" ref="D4:D18" si="0">3.3*C4/1023</f>
+        <v>0.70645161290322578</v>
+      </c>
+      <c r="E4">
         <v>-74.5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0.6</v>
       </c>
@@ -7439,16 +9636,20 @@
         <v>295</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.95161290322580649</v>
+      </c>
+      <c r="E5">
         <v>-72.599999999999994</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.8</v>
       </c>
@@ -7456,16 +9657,20 @@
         <v>381</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.2290322580645161</v>
+      </c>
+      <c r="E6">
         <v>-70.900000000000006</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -7473,16 +9678,20 @@
         <v>483</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.5580645161290321</v>
+      </c>
+      <c r="E7">
         <v>-69.400000000000006</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.2</v>
       </c>
@@ -7490,16 +9699,20 @@
         <v>592</v>
       </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.9096774193548387</v>
+      </c>
+      <c r="E8">
         <v>-68.099999999999994</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -7507,16 +9720,20 @@
         <v>687</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.2161290322580642</v>
+      </c>
+      <c r="E9">
         <v>-67</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.5</v>
       </c>
@@ -7524,16 +9741,20 @@
         <v>730</v>
       </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.3548387096774195</v>
+      </c>
+      <c r="E10">
         <v>-66.3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1.6</v>
       </c>
@@ -7541,16 +9762,20 @@
         <v>766</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.4709677419354836</v>
+      </c>
+      <c r="E11">
         <v>-65.8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1.8</v>
       </c>
@@ -7558,16 +9783,20 @@
         <v>822</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2.6516129032258062</v>
+      </c>
+      <c r="E12">
         <v>-64.8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2</v>
       </c>
@@ -7575,16 +9804,20 @@
         <v>864</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2.7870967741935484</v>
+      </c>
+      <c r="E13">
         <v>-63.9</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2.2000000000000002</v>
       </c>
@@ -7592,16 +9825,20 @@
         <v>884</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2.8516129032258064</v>
+      </c>
+      <c r="E14">
         <v>-63.1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.4</v>
       </c>
@@ -7609,16 +9846,20 @@
         <v>882</v>
       </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>2.8451612903225807</v>
+      </c>
+      <c r="E15">
         <v>-62.3</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2.6</v>
       </c>
@@ -7626,16 +9867,20 @@
         <v>880</v>
       </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>2.838709677419355</v>
+      </c>
+      <c r="E16">
         <v>-61.6</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2.8</v>
       </c>
@@ -7643,16 +9888,20 @@
         <v>880</v>
       </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>2.838709677419355</v>
+      </c>
+      <c r="E17">
         <v>-60.8</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>12</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3</v>
       </c>
@@ -7660,12 +9909,16 @@
         <v>880</v>
       </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2.838709677419355</v>
+      </c>
+      <c r="E18">
         <v>-60.2</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7679,8 +9932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431D0629-441B-4A6C-8F34-63C06F1A2AF1}">
   <dimension ref="B2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J18"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7789,7 +10042,7 @@
         <v>-24.979999999999997</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I3:I17" si="3">$C$20*D4</f>
+        <f t="shared" ref="I4:I17" si="3">$C$20*D4</f>
         <v>177.36465429251882</v>
       </c>
       <c r="J4">

</xml_diff>

<commit_message>
Add support to correct (saturation) and calculate waveguide power, minor fixes in v5019, more power values measured.
</commit_message>
<xml_diff>
--- a/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
+++ b/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matro\Documents\AIUC\Scripts\RFLabTests\rf_measures_powervoltage_curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B542FC56-D2D0-4ED0-825E-FCD34D7F4398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3995B1AA-0E76-48CB-9951-C4F5F5D85DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ajuste 14-15 dec" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">Total_fix!$K$19</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Total_fix!$P$19</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>Voltage Attenuation</t>
   </si>
@@ -159,6 +159,21 @@
   <si>
     <t>ADC measured (in Volts)</t>
   </si>
+  <si>
+    <t>ADC new in volts</t>
+  </si>
+  <si>
+    <t>ADC old scaled in Volts</t>
+  </si>
+  <si>
+    <t>ADC new - old scaled</t>
+  </si>
+  <si>
+    <t>Corrected power Measured (03/03) (dBm)</t>
+  </si>
+  <si>
+    <t>Corrected power waveguide (03/03) (dBm)</t>
+  </si>
 </sst>
 </file>
 
@@ -173,12 +188,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,8 +214,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2438,7 +2460,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Total_fix!$I$2</c:f>
+              <c:f>Total_fix!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2530,7 +2552,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Total_fix!$I$3:$I$18</c:f>
+              <c:f>Total_fix!$K$3:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2597,7 +2619,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Total_fix!$J$2</c:f>
+              <c:f>Total_fix!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2689,7 +2711,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Total_fix!$J$3:$J$18</c:f>
+              <c:f>Total_fix!$L$3:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3295,7 +3317,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Total_fix!$G$3,Total_fix!$H$3,Total_fix!$G$4,Total_fix!$H$4,Total_fix!$G$5,Total_fix!$H$5,Total_fix!$G$6,Total_fix!$H$6,Total_fix!$G$7,Total_fix!$H$7,Total_fix!$G$8,Total_fix!$H$8,Total_fix!$G$9,Total_fix!$H$9,Total_fix!$G$10,Total_fix!$H$10,Total_fix!$G$11,Total_fix!$H$11,Total_fix!$G$12,Total_fix!$H$12,Total_fix!$G$13,Total_fix!$H$13,Total_fix!$G$14,Total_fix!$H$14,Total_fix!$G$15,Total_fix!$H$15,Total_fix!$G$16,Total_fix!$H$16,Total_fix!$G$17,Total_fix!$H$17,Total_fix!$G$18,Total_fix!$H$18)</c:f>
+              <c:f>(Total_fix!$H$3,Total_fix!$I$3,Total_fix!$H$4,Total_fix!$I$4,Total_fix!$H$5,Total_fix!$I$5,Total_fix!$H$6,Total_fix!$I$6,Total_fix!$H$7,Total_fix!$I$7,Total_fix!$H$8,Total_fix!$I$8,Total_fix!$H$9,Total_fix!$I$9,Total_fix!$H$10,Total_fix!$I$10,Total_fix!$H$11,Total_fix!$I$11,Total_fix!$H$12,Total_fix!$I$12,Total_fix!$H$13,Total_fix!$I$13,Total_fix!$H$14,Total_fix!$I$14,Total_fix!$H$15,Total_fix!$I$15,Total_fix!$H$16,Total_fix!$I$16,Total_fix!$H$17,Total_fix!$I$17,Total_fix!$H$18,Total_fix!$I$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -3410,7 +3432,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Total_fix!$G$2</c:f>
+              <c:f>Total_fix!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3502,7 +3524,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Total_fix!$G$3:$G$18</c:f>
+              <c:f>Total_fix!$H$3:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3569,7 +3591,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Total_fix!$H$2</c:f>
+              <c:f>Total_fix!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3661,7 +3683,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Total_fix!$H$3:$H$18</c:f>
+              <c:f>Total_fix!$I$3:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -3720,6 +3742,165 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-455E-4F2B-A1D6-5FA54704DC9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Corrected power waveguide (03/03) (dBm)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$J$3:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-27.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-23.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-22.080000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20.580000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-19.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-18.080000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-17.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-16.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-15.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-14.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-14.280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13.579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-12.579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-11.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-11.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CC55-4AF6-B286-5AEC927BBE2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4328,7 +4509,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Total_fix!$G$3,Total_fix!$H$3,Total_fix!$G$4,Total_fix!$H$4,Total_fix!$G$5,Total_fix!$H$5,Total_fix!$G$6,Total_fix!$H$6,Total_fix!$G$7,Total_fix!$H$7,Total_fix!$G$8,Total_fix!$H$8,Total_fix!$G$9,Total_fix!$H$9,Total_fix!$G$10,Total_fix!$H$10,Total_fix!$G$11,Total_fix!$H$11,Total_fix!$G$12,Total_fix!$H$12,Total_fix!$G$13,Total_fix!$H$13,Total_fix!$G$14,Total_fix!$H$14,Total_fix!$G$15,Total_fix!$H$15,Total_fix!$G$16,Total_fix!$H$16,Total_fix!$G$17,Total_fix!$H$17,Total_fix!$G$18,Total_fix!$H$18)</c:f>
+              <c:f>(Total_fix!$H$3,Total_fix!$I$3,Total_fix!$H$4,Total_fix!$I$4,Total_fix!$H$5,Total_fix!$I$5,Total_fix!$H$6,Total_fix!$I$6,Total_fix!$H$7,Total_fix!$I$7,Total_fix!$H$8,Total_fix!$I$8,Total_fix!$H$9,Total_fix!$I$9,Total_fix!$H$10,Total_fix!$I$10,Total_fix!$H$11,Total_fix!$I$11,Total_fix!$H$12,Total_fix!$I$12,Total_fix!$H$13,Total_fix!$I$13,Total_fix!$H$14,Total_fix!$I$14,Total_fix!$H$15,Total_fix!$I$15,Total_fix!$H$16,Total_fix!$I$16,Total_fix!$H$17,Total_fix!$I$17,Total_fix!$H$18,Total_fix!$I$18)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -4690,6 +4871,1658 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1121015040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>ADC </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CL" baseline="0"/>
+              <a:t>vs Voltage input</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC new measured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$D$3:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7306-4933-80B6-2C47DFCD9183}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC old scaled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$L$3:$L$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>87.142503457927859</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118.53545501420001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>159.6710467086256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>206.21921625758085</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>261.4275103737836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320.4246089881571</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>371.84409860618911</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>395.11818338066672</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>414.60346365697359</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>444.9138996423398</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>467.64672663136446</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>478.4718823404238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>477.38936676951784</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>476.30685119861192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>476.30685119861192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>476.30685119861192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7306-4933-80B6-2C47DFCD9183}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="724192031"/>
+        <c:axId val="724192447"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="724192031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724192447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="724192447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724192031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Voltage ADC scaled</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CL" baseline="0"/>
+              <a:t> vs Voltage Input</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC new in volts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$M$3:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.20645161290322581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30967741935483867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46129032258064512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61935483870967734</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82258064516129037</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0419354838709676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2774193548387096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4193548387096775</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5290322580645159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7806451612903225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0161290322580645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2193548387096773</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3838709677419354</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5290322580645159</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6451612903225805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7483870967741932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0884-46C4-A148-909851535CC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC old scaled in Volts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$N$3:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.28110484986428341</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38237243552967748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51506789260846964</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66522327825026073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.84331454959285024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0336277709295389</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1994970922780293</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2745747850989246</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3374305279257213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4352061278785153</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5085378278431112</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5434576849691088</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5399656992565092</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5364737135439095</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5364737135439095</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5364737135439095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0884-46C4-A148-909851535CC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Total_fix!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC new - old scaled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$O$3:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-7.4653236961057606E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.2695016174838811E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.3777570027824517E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.5868439540583394E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.0733904431559869E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3077129414286244E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7922262560680355E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14478005361075286</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19160173013879467</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34543903341180715</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50759120441495331</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.67589715374056847</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84390526848542624</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99255854452060643</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.108687576778671</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2119133832302837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0884-46C4-A148-909851535CC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>ADC diff non saturated zone</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$O$3:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-7.4653236961057606E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.2695016174838811E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.3777570027824517E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.5868439540583394E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.0733904431559869E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3077129414286244E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0884-46C4-A148-909851535CC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>ADC diff saturated zone</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11044747455348569"/>
+                  <c:y val="0.12669833274889222"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Total_fix!$B$8:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Total_fix!$O$8:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.3077129414286244E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7922262560680355E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14478005361075286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19160173013879467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34543903341180715</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.50759120441495331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67589715374056847</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84390526848542624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99255854452060643</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.108687576778671</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2119133832302837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0884-46C4-A148-909851535CC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="721898799"/>
+        <c:axId val="721899215"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="721898799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="721899215"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="721899215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="721898799"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5056,6 +6889,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8153,6 +10066,1038 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8870,7 +11815,7 @@
       <xdr:rowOff>13834</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1271683</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>13835</xdr:rowOff>
@@ -8900,13 +11845,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>24450</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>26080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>162995</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>26081</xdr:rowOff>
@@ -8931,6 +11876,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1021080</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FBF0F71-9CAE-435C-AA10-786E5A83BA5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1402080</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7188E7BD-8935-4002-B0BC-B709ACFA060F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9562,7 +12579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501F32F7-C9D6-47EE-A900-3F721E2AB069}">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
@@ -9930,10 +12947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431D0629-441B-4A6C-8F34-63C06F1A2AF1}">
-  <dimension ref="B2:K21"/>
+  <dimension ref="B2:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9941,14 +12958,16 @@
     <col min="2" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -9965,22 +12984,37 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0.2</v>
       </c>
@@ -9997,27 +13031,46 @@
         <v>-75.900000000000006</v>
       </c>
       <c r="G3">
+        <v>-76.8</v>
+      </c>
+      <c r="H3">
         <f>E3+$C$21</f>
         <v>-28.080000000000005</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <f>$C$21+F3</f>
         <v>-27.080000000000005</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <f>G3+$C$21</f>
+        <v>-27.979999999999997</v>
+      </c>
+      <c r="K3">
         <f>$C$20*D3</f>
         <v>118.2431028616792</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <f>(1/$C$20)*C3</f>
         <v>87.142503457927859</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K9" si="0">(C3-$C$20*D3)^2</f>
+      <c r="M3" s="1">
+        <f>D3*3.3/1023</f>
+        <v>0.20645161290322581</v>
+      </c>
+      <c r="N3" s="1">
+        <f>L3*3.3/1023</f>
+        <v>0.28110484986428341</v>
+      </c>
+      <c r="O3" s="1">
+        <f>M3-N3</f>
+        <v>-7.4653236961057606E-2</v>
+      </c>
+      <c r="P3">
+        <f>(C3-$C$20*D3)^2</f>
         <v>1828.1522528969449</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0.4</v>
       </c>
@@ -10034,27 +13087,46 @@
         <v>-73.8</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G18" si="1">E4+$C$21</f>
+        <v>-74.7</v>
+      </c>
+      <c r="H4">
+        <f>E4+$C$21</f>
         <v>-25.68</v>
       </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H18" si="2">$C$21+F4</f>
+      <c r="I4">
+        <f>$C$21+F4</f>
         <v>-24.979999999999997</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I17" si="3">$C$20*D4</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J18" si="0">G4+$C$21</f>
+        <v>-25.880000000000003</v>
+      </c>
+      <c r="K4">
+        <f>$C$20*D4</f>
         <v>177.36465429251882</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J18" si="4">(1/$C$20)*C4</f>
+      <c r="L4">
+        <f>(1/$C$20)*C4</f>
         <v>118.53545501420001</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
+      <c r="M4" s="1">
+        <f>D4*3.3/1023</f>
+        <v>0.30967741935483867</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N18" si="1">L4*3.3/1023</f>
+        <v>0.38237243552967748</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O18" si="2">M4-N4</f>
+        <v>-7.2695016174838811E-2</v>
+      </c>
+      <c r="P4">
+        <f>(C4-$C$20*D4)^2</f>
         <v>1733.5020121814714</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0.6</v>
       </c>
@@ -10071,27 +13143,46 @@
         <v>-71.8</v>
       </c>
       <c r="G5">
+        <v>-72.5</v>
+      </c>
+      <c r="H5">
+        <f>E5+$C$21</f>
+        <v>-23.779999999999994</v>
+      </c>
+      <c r="I5">
+        <f>$C$21+F5</f>
+        <v>-22.979999999999997</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-23.68</v>
+      </c>
+      <c r="K5">
+        <f>$C$20*D5</f>
+        <v>264.19943295656446</v>
+      </c>
+      <c r="L5">
+        <f>(1/$C$20)*C5</f>
+        <v>159.6710467086256</v>
+      </c>
+      <c r="M5" s="1">
+        <f>D5*3.3/1023</f>
+        <v>0.46129032258064512</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="1"/>
-        <v>-23.779999999999994</v>
-      </c>
-      <c r="H5">
+        <v>0.51506789260846964</v>
+      </c>
+      <c r="O5" s="1">
         <f t="shared" si="2"/>
-        <v>-22.979999999999997</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="3"/>
-        <v>264.19943295656446</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="4"/>
-        <v>159.6710467086256</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
+        <v>-5.3777570027824517E-2</v>
+      </c>
+      <c r="P5">
+        <f>(C5-$C$20*D5)^2</f>
         <v>948.67493019716721</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.8</v>
       </c>
@@ -10108,27 +13199,46 @@
         <v>-70.2</v>
       </c>
       <c r="G6">
+        <v>-70.900000000000006</v>
+      </c>
+      <c r="H6">
+        <f>E6+$C$21</f>
+        <v>-22.080000000000005</v>
+      </c>
+      <c r="I6">
+        <f>$C$21+F6</f>
+        <v>-21.380000000000003</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-22.080000000000005</v>
+      </c>
+      <c r="K6">
+        <f>$C$20*D6</f>
+        <v>354.72930858503764</v>
+      </c>
+      <c r="L6">
+        <f>(1/$C$20)*C6</f>
+        <v>206.21921625758085</v>
+      </c>
+      <c r="M6" s="1">
+        <f>D6*3.3/1023</f>
+        <v>0.61935483870967734</v>
+      </c>
+      <c r="N6" s="1">
         <f t="shared" si="1"/>
-        <v>-22.080000000000005</v>
-      </c>
-      <c r="H6">
+        <v>0.66522327825026073</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" si="2"/>
-        <v>-21.380000000000003</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="3"/>
-        <v>354.72930858503764</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="4"/>
-        <v>206.21921625758085</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+        <v>-4.5868439540583394E-2</v>
+      </c>
+      <c r="P6">
+        <f>(C6-$C$20*D6)^2</f>
         <v>690.14922742017689</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -10145,27 +13255,46 @@
         <v>-68.599999999999994</v>
       </c>
       <c r="G7">
+        <v>-69.400000000000006</v>
+      </c>
+      <c r="H7">
+        <f>E7+$C$21</f>
+        <v>-20.580000000000005</v>
+      </c>
+      <c r="I7">
+        <f>$C$21+F7</f>
+        <v>-19.779999999999994</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>-20.580000000000005</v>
+      </c>
+      <c r="K7">
+        <f>$C$20*D7</f>
+        <v>471.12486296450311</v>
+      </c>
+      <c r="L7">
+        <f>(1/$C$20)*C7</f>
+        <v>261.4275103737836</v>
+      </c>
+      <c r="M7" s="1">
+        <f>D7*3.3/1023</f>
+        <v>0.82258064516129037</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="1"/>
-        <v>-20.580000000000005</v>
-      </c>
-      <c r="H7">
+        <v>0.84331454959285024</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" si="2"/>
-        <v>-19.779999999999994</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
-        <v>471.12486296450311</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="4"/>
-        <v>261.4275103737836</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
+        <v>-2.0733904431559869E-2</v>
+      </c>
+      <c r="P7">
+        <f>(C7-$C$20*D7)^2</f>
         <v>141.0188796118299</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1.2</v>
       </c>
@@ -10182,27 +13311,46 @@
         <v>-67.3</v>
       </c>
       <c r="G8">
+        <v>-68</v>
+      </c>
+      <c r="H8">
+        <f>E8+$C$21</f>
+        <v>-19.279999999999994</v>
+      </c>
+      <c r="I8">
+        <f>$C$21+F8</f>
+        <v>-18.479999999999997</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>-19.18</v>
+      </c>
+      <c r="K8">
+        <f>$C$20*D8</f>
+        <v>596.75815975503724</v>
+      </c>
+      <c r="L8">
+        <f>(1/$C$20)*C8</f>
+        <v>320.4246089881571</v>
+      </c>
+      <c r="M8" s="1">
+        <f>D8*3.3/1023</f>
+        <v>1.0419354838709676</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="1"/>
-        <v>-19.279999999999994</v>
-      </c>
-      <c r="H8">
+        <v>1.0336277709295389</v>
+      </c>
+      <c r="O8" s="1">
         <f t="shared" si="2"/>
-        <v>-18.479999999999997</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="3"/>
-        <v>596.75815975503724</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="4"/>
-        <v>320.4246089881571</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
+        <v>8.3077129414286244E-3</v>
+      </c>
+      <c r="P8">
+        <f>(C8-$C$20*D8)^2</f>
         <v>22.640084254456056</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1.4</v>
       </c>
@@ -10219,27 +13367,46 @@
         <v>-66.099999999999994</v>
       </c>
       <c r="G9">
+        <v>-66.900000000000006</v>
+      </c>
+      <c r="H9">
+        <f>E9+$C$21</f>
+        <v>-18.18</v>
+      </c>
+      <c r="I9">
+        <f>$C$21+F9</f>
+        <v>-17.279999999999994</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>-18.080000000000005</v>
+      </c>
+      <c r="K9">
+        <f>$C$20*D9</f>
+        <v>731.62919895664004</v>
+      </c>
+      <c r="L9">
+        <f>(1/$C$20)*C9</f>
+        <v>371.84409860618911</v>
+      </c>
+      <c r="M9" s="1">
+        <f>D9*3.3/1023</f>
+        <v>1.2774193548387096</v>
+      </c>
+      <c r="N9" s="1">
         <f t="shared" si="1"/>
-        <v>-18.18</v>
-      </c>
-      <c r="H9">
+        <v>1.1994970922780293</v>
+      </c>
+      <c r="O9" s="1">
         <f t="shared" si="2"/>
-        <v>-17.279999999999994</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>731.62919895664004</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="4"/>
-        <v>371.84409860618911</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
+        <v>7.7922262560680355E-2</v>
+      </c>
+      <c r="P9">
+        <f>(C9-$C$20*D9)^2</f>
         <v>1991.7653995113603</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1.5</v>
       </c>
@@ -10256,23 +13423,42 @@
         <v>-65.5</v>
       </c>
       <c r="G10">
+        <v>-66.3</v>
+      </c>
+      <c r="H10">
+        <f>E10+$C$21</f>
+        <v>-17.479999999999997</v>
+      </c>
+      <c r="I10">
+        <f>$C$21+F10</f>
+        <v>-16.68</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>-17.479999999999997</v>
+      </c>
+      <c r="K10">
+        <f>$C$20*D10</f>
+        <v>812.92133217404455</v>
+      </c>
+      <c r="L10">
+        <f>(1/$C$20)*C10</f>
+        <v>395.11818338066672</v>
+      </c>
+      <c r="M10" s="1">
+        <f>D10*3.3/1023</f>
+        <v>1.4193548387096775</v>
+      </c>
+      <c r="N10" s="1">
         <f t="shared" si="1"/>
-        <v>-17.479999999999997</v>
-      </c>
-      <c r="H10">
+        <v>1.2745747850989246</v>
+      </c>
+      <c r="O10" s="1">
         <f t="shared" si="2"/>
-        <v>-16.68</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="3"/>
-        <v>812.92133217404455</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="4"/>
-        <v>395.11818338066672</v>
+        <v>0.14478005361075286</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>1.6</v>
       </c>
@@ -10289,23 +13475,42 @@
         <v>-65.099999999999994</v>
       </c>
       <c r="G11">
+        <v>-65.8</v>
+      </c>
+      <c r="H11">
+        <f>E11+$C$21</f>
+        <v>-16.979999999999997</v>
+      </c>
+      <c r="I11">
+        <f>$C$21+F11</f>
+        <v>-16.279999999999994</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-16.979999999999997</v>
+      </c>
+      <c r="K11">
+        <f>$C$20*D11</f>
+        <v>875.73798056931162</v>
+      </c>
+      <c r="L11">
+        <f>(1/$C$20)*C11</f>
+        <v>414.60346365697359</v>
+      </c>
+      <c r="M11" s="1">
+        <f>D11*3.3/1023</f>
+        <v>1.5290322580645159</v>
+      </c>
+      <c r="N11" s="1">
         <f t="shared" si="1"/>
-        <v>-16.979999999999997</v>
-      </c>
-      <c r="H11">
+        <v>1.3374305279257213</v>
+      </c>
+      <c r="O11" s="1">
         <f t="shared" si="2"/>
-        <v>-16.279999999999994</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>875.73798056931162</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="4"/>
-        <v>414.60346365697359</v>
+        <v>0.19160173013879467</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1.8</v>
       </c>
@@ -10322,23 +13527,42 @@
         <v>-64.099999999999994</v>
       </c>
       <c r="G12">
+        <v>-64.7</v>
+      </c>
+      <c r="H12">
+        <f>E12+$C$21</f>
+        <v>-15.979999999999997</v>
+      </c>
+      <c r="I12">
+        <f>$C$21+F12</f>
+        <v>-15.279999999999994</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-15.880000000000003</v>
+      </c>
+      <c r="K12">
+        <f>$C$20*D12</f>
+        <v>1019.8467621819832</v>
+      </c>
+      <c r="L12">
+        <f>(1/$C$20)*C12</f>
+        <v>444.9138996423398</v>
+      </c>
+      <c r="M12" s="1">
+        <f>D12*3.3/1023</f>
+        <v>1.7806451612903225</v>
+      </c>
+      <c r="N12" s="1">
         <f t="shared" si="1"/>
-        <v>-15.979999999999997</v>
-      </c>
-      <c r="H12">
+        <v>1.4352061278785153</v>
+      </c>
+      <c r="O12" s="1">
         <f t="shared" si="2"/>
-        <v>-15.279999999999994</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="3"/>
-        <v>1019.8467621819832</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="4"/>
-        <v>444.9138996423398</v>
+        <v>0.34543903341180715</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2</v>
       </c>
@@ -10355,23 +13579,42 @@
         <v>-63.2</v>
       </c>
       <c r="G13">
+        <v>-63.8</v>
+      </c>
+      <c r="H13">
+        <f>E13+$C$21</f>
+        <v>-15.079999999999998</v>
+      </c>
+      <c r="I13">
+        <f>$C$21+F13</f>
+        <v>-14.380000000000003</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>-14.979999999999997</v>
+      </c>
+      <c r="K13">
+        <f>$C$20*D13</f>
+        <v>1154.717801383586</v>
+      </c>
+      <c r="L13">
+        <f>(1/$C$20)*C13</f>
+        <v>467.64672663136446</v>
+      </c>
+      <c r="M13" s="1">
+        <f>D13*3.3/1023</f>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="N13" s="1">
         <f t="shared" si="1"/>
-        <v>-15.079999999999998</v>
-      </c>
-      <c r="H13">
+        <v>1.5085378278431112</v>
+      </c>
+      <c r="O13" s="1">
         <f t="shared" si="2"/>
-        <v>-14.380000000000003</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
-        <v>1154.717801383586</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="4"/>
-        <v>467.64672663136446</v>
+        <v>0.50759120441495331</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2.2000000000000002</v>
       </c>
@@ -10388,23 +13631,42 @@
         <v>-62.3</v>
       </c>
       <c r="G14">
+        <v>-63.1</v>
+      </c>
+      <c r="H14">
+        <f>E14+$C$21</f>
+        <v>-14.280000000000001</v>
+      </c>
+      <c r="I14">
+        <f>$C$21+F14</f>
+        <v>-13.479999999999997</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-14.280000000000001</v>
+      </c>
+      <c r="K14">
+        <f>$C$20*D14</f>
+        <v>1271.1133557630515</v>
+      </c>
+      <c r="L14">
+        <f>(1/$C$20)*C14</f>
+        <v>478.4718823404238</v>
+      </c>
+      <c r="M14" s="1">
+        <f>D14*3.3/1023</f>
+        <v>2.2193548387096773</v>
+      </c>
+      <c r="N14" s="1">
         <f t="shared" si="1"/>
-        <v>-14.280000000000001</v>
-      </c>
-      <c r="H14">
+        <v>1.5434576849691088</v>
+      </c>
+      <c r="O14" s="1">
         <f t="shared" si="2"/>
-        <v>-13.479999999999997</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
-        <v>1271.1133557630515</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="4"/>
-        <v>478.4718823404238</v>
+        <v>0.67589715374056847</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2.4</v>
       </c>
@@ -10421,23 +13683,42 @@
         <v>-61.6</v>
       </c>
       <c r="G15">
+        <v>-62.4</v>
+      </c>
+      <c r="H15">
+        <f>E15+$C$21</f>
+        <v>-13.479999999999997</v>
+      </c>
+      <c r="I15">
+        <f>$C$21+F15</f>
+        <v>-12.780000000000001</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>-13.579999999999998</v>
+      </c>
+      <c r="K15">
+        <f>$C$20*D15</f>
+        <v>1365.3383283559522</v>
+      </c>
+      <c r="L15">
+        <f>(1/$C$20)*C15</f>
+        <v>477.38936676951784</v>
+      </c>
+      <c r="M15" s="1">
+        <f>D15*3.3/1023</f>
+        <v>2.3838709677419354</v>
+      </c>
+      <c r="N15" s="1">
         <f t="shared" si="1"/>
-        <v>-13.479999999999997</v>
-      </c>
-      <c r="H15">
+        <v>1.5399656992565092</v>
+      </c>
+      <c r="O15" s="1">
         <f t="shared" si="2"/>
-        <v>-12.780000000000001</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
-        <v>1365.3383283559522</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="4"/>
-        <v>477.38936676951784</v>
+        <v>0.84390526848542624</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2.6</v>
       </c>
@@ -10454,23 +13735,42 @@
         <v>-61.1</v>
       </c>
       <c r="G16">
+        <v>-61.4</v>
+      </c>
+      <c r="H16">
+        <f>E16+$C$21</f>
+        <v>-12.780000000000001</v>
+      </c>
+      <c r="I16">
+        <f>$C$21+F16</f>
+        <v>-12.280000000000001</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>-12.579999999999998</v>
+      </c>
+      <c r="K16">
+        <f>$C$20*D16</f>
+        <v>1448.4780100555702</v>
+      </c>
+      <c r="L16">
+        <f>(1/$C$20)*C16</f>
+        <v>476.30685119861192</v>
+      </c>
+      <c r="M16" s="1">
+        <f>D16*3.3/1023</f>
+        <v>2.5290322580645159</v>
+      </c>
+      <c r="N16" s="1">
         <f t="shared" si="1"/>
-        <v>-12.780000000000001</v>
-      </c>
-      <c r="H16">
+        <v>1.5364737135439095</v>
+      </c>
+      <c r="O16" s="1">
         <f t="shared" si="2"/>
-        <v>-12.280000000000001</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
-        <v>1448.4780100555702</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="4"/>
-        <v>476.30685119861192</v>
+        <v>0.99255854452060643</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2.8</v>
       </c>
@@ -10487,23 +13787,42 @@
         <v>-60.4</v>
       </c>
       <c r="G17">
+        <v>-60.7</v>
+      </c>
+      <c r="H17">
+        <f>E17+$C$21</f>
+        <v>-11.979999999999997</v>
+      </c>
+      <c r="I17">
+        <f>$C$21+F17</f>
+        <v>-11.579999999999998</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>-11.880000000000003</v>
+      </c>
+      <c r="K17">
+        <f>$C$20*D17</f>
+        <v>1514.9897554152649</v>
+      </c>
+      <c r="L17">
+        <f>(1/$C$20)*C17</f>
+        <v>476.30685119861192</v>
+      </c>
+      <c r="M17" s="1">
+        <f>D17*3.3/1023</f>
+        <v>2.6451612903225805</v>
+      </c>
+      <c r="N17" s="1">
         <f t="shared" si="1"/>
-        <v>-11.979999999999997</v>
-      </c>
-      <c r="H17">
+        <v>1.5364737135439095</v>
+      </c>
+      <c r="O17" s="1">
         <f t="shared" si="2"/>
-        <v>-11.579999999999998</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="3"/>
-        <v>1514.9897554152649</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="4"/>
-        <v>476.30685119861192</v>
+        <v>1.108687576778671</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3</v>
       </c>
@@ -10520,29 +13839,48 @@
         <v>-59.8</v>
       </c>
       <c r="G18">
+        <v>-60</v>
+      </c>
+      <c r="H18">
+        <f>E18+$C$21</f>
+        <v>-11.380000000000003</v>
+      </c>
+      <c r="I18">
+        <f>$C$21+F18</f>
+        <v>-10.979999999999997</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>-11.18</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18" si="3">$C$20*D18</f>
+        <v>1574.1113068461045</v>
+      </c>
+      <c r="L18">
+        <f>(1/$C$20)*C18</f>
+        <v>476.30685119861192</v>
+      </c>
+      <c r="M18" s="1">
+        <f>D18*3.3/1023</f>
+        <v>2.7483870967741932</v>
+      </c>
+      <c r="N18" s="1">
         <f t="shared" si="1"/>
-        <v>-11.380000000000003</v>
-      </c>
-      <c r="H18">
+        <v>1.5364737135439095</v>
+      </c>
+      <c r="O18" s="1">
         <f t="shared" si="2"/>
-        <v>-10.979999999999997</v>
-      </c>
-      <c r="I18">
-        <f t="shared" ref="I18" si="5">$C$20*D18</f>
-        <v>1574.1113068461045</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="4"/>
-        <v>476.30685119861192</v>
+        <v>1.2119133832302837</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K19">
-        <f>SUM(K3:K9)</f>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <f>SUM(P3:P9)</f>
         <v>7355.9027860734068</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -10550,7 +13888,7 @@
         <v>1.8475484822137376</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Change adc to dBm power conversion values, and minor improvements to plots.
</commit_message>
<xml_diff>
--- a/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
+++ b/rf_measures_powervoltage_curve/voltage_power_curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matro\Documents\AIUC\Scripts\RFLabTests\rf_measures_powervoltage_curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3995B1AA-0E76-48CB-9951-C4F5F5D85DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731A5E17-2A38-4BE2-B248-30BC12519B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ajuste 14-15 dec" sheetId="1" r:id="rId1"/>
@@ -12221,7 +12221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -12949,7 +12949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431D0629-441B-4A6C-8F34-63C06F1A2AF1}">
   <dimension ref="B2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -13034,11 +13034,11 @@
         <v>-76.8</v>
       </c>
       <c r="H3">
-        <f>E3+$C$21</f>
+        <f t="shared" ref="H3:H18" si="0">E3+$C$21</f>
         <v>-28.080000000000005</v>
       </c>
       <c r="I3">
-        <f>$C$21+F3</f>
+        <f t="shared" ref="I3:I18" si="1">$C$21+F3</f>
         <v>-27.080000000000005</v>
       </c>
       <c r="J3">
@@ -13046,15 +13046,15 @@
         <v>-27.979999999999997</v>
       </c>
       <c r="K3">
-        <f>$C$20*D3</f>
+        <f t="shared" ref="K3:K17" si="2">$C$20*D3</f>
         <v>118.2431028616792</v>
       </c>
       <c r="L3">
-        <f>(1/$C$20)*C3</f>
+        <f t="shared" ref="L3:L18" si="3">(1/$C$20)*C3</f>
         <v>87.142503457927859</v>
       </c>
       <c r="M3" s="1">
-        <f>D3*3.3/1023</f>
+        <f t="shared" ref="M3:M18" si="4">D3*3.3/1023</f>
         <v>0.20645161290322581</v>
       </c>
       <c r="N3" s="1">
@@ -13066,7 +13066,7 @@
         <v>-7.4653236961057606E-2</v>
       </c>
       <c r="P3">
-        <f>(C3-$C$20*D3)^2</f>
+        <f t="shared" ref="P3:P9" si="5">(C3-$C$20*D3)^2</f>
         <v>1828.1522528969449</v>
       </c>
     </row>
@@ -13090,39 +13090,39 @@
         <v>-74.7</v>
       </c>
       <c r="H4">
-        <f>E4+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-25.68</v>
       </c>
       <c r="I4">
-        <f>$C$21+F4</f>
+        <f t="shared" si="1"/>
         <v>-24.979999999999997</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J18" si="0">G4+$C$21</f>
+        <f t="shared" ref="J4:J18" si="6">G4+$C$21</f>
         <v>-25.880000000000003</v>
       </c>
       <c r="K4">
-        <f>$C$20*D4</f>
+        <f t="shared" si="2"/>
         <v>177.36465429251882</v>
       </c>
       <c r="L4">
-        <f>(1/$C$20)*C4</f>
+        <f t="shared" si="3"/>
         <v>118.53545501420001</v>
       </c>
       <c r="M4" s="1">
-        <f>D4*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>0.30967741935483867</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N18" si="1">L4*3.3/1023</f>
+        <f t="shared" ref="N4:N18" si="7">L4*3.3/1023</f>
         <v>0.38237243552967748</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O18" si="2">M4-N4</f>
+        <f t="shared" ref="O4:O18" si="8">M4-N4</f>
         <v>-7.2695016174838811E-2</v>
       </c>
       <c r="P4">
-        <f>(C4-$C$20*D4)^2</f>
+        <f t="shared" si="5"/>
         <v>1733.5020121814714</v>
       </c>
     </row>
@@ -13146,39 +13146,39 @@
         <v>-72.5</v>
       </c>
       <c r="H5">
-        <f>E5+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-23.779999999999994</v>
       </c>
       <c r="I5">
-        <f>$C$21+F5</f>
+        <f t="shared" si="1"/>
         <v>-22.979999999999997</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-23.68</v>
       </c>
       <c r="K5">
-        <f>$C$20*D5</f>
+        <f t="shared" si="2"/>
         <v>264.19943295656446</v>
       </c>
       <c r="L5">
-        <f>(1/$C$20)*C5</f>
+        <f t="shared" si="3"/>
         <v>159.6710467086256</v>
       </c>
       <c r="M5" s="1">
-        <f>D5*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>0.46129032258064512</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.51506789260846964</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>-5.3777570027824517E-2</v>
       </c>
       <c r="P5">
-        <f>(C5-$C$20*D5)^2</f>
+        <f t="shared" si="5"/>
         <v>948.67493019716721</v>
       </c>
     </row>
@@ -13202,39 +13202,39 @@
         <v>-70.900000000000006</v>
       </c>
       <c r="H6">
-        <f>E6+$C$21</f>
-        <v>-22.080000000000005</v>
-      </c>
-      <c r="I6">
-        <f>$C$21+F6</f>
-        <v>-21.380000000000003</v>
-      </c>
-      <c r="J6">
         <f t="shared" si="0"/>
         <v>-22.080000000000005</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-21.380000000000003</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="6"/>
+        <v>-22.080000000000005</v>
+      </c>
       <c r="K6">
-        <f>$C$20*D6</f>
+        <f t="shared" si="2"/>
         <v>354.72930858503764</v>
       </c>
       <c r="L6">
-        <f>(1/$C$20)*C6</f>
+        <f t="shared" si="3"/>
         <v>206.21921625758085</v>
       </c>
       <c r="M6" s="1">
-        <f>D6*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>0.61935483870967734</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.66522327825026073</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>-4.5868439540583394E-2</v>
       </c>
       <c r="P6">
-        <f>(C6-$C$20*D6)^2</f>
+        <f t="shared" si="5"/>
         <v>690.14922742017689</v>
       </c>
     </row>
@@ -13258,39 +13258,39 @@
         <v>-69.400000000000006</v>
       </c>
       <c r="H7">
-        <f>E7+$C$21</f>
-        <v>-20.580000000000005</v>
-      </c>
-      <c r="I7">
-        <f>$C$21+F7</f>
-        <v>-19.779999999999994</v>
-      </c>
-      <c r="J7">
         <f t="shared" si="0"/>
         <v>-20.580000000000005</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>-19.779999999999994</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>-20.580000000000005</v>
+      </c>
       <c r="K7">
-        <f>$C$20*D7</f>
+        <f t="shared" si="2"/>
         <v>471.12486296450311</v>
       </c>
       <c r="L7">
-        <f>(1/$C$20)*C7</f>
+        <f t="shared" si="3"/>
         <v>261.4275103737836</v>
       </c>
       <c r="M7" s="1">
-        <f>D7*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>0.82258064516129037</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.84331454959285024</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>-2.0733904431559869E-2</v>
       </c>
       <c r="P7">
-        <f>(C7-$C$20*D7)^2</f>
+        <f t="shared" si="5"/>
         <v>141.0188796118299</v>
       </c>
     </row>
@@ -13314,39 +13314,39 @@
         <v>-68</v>
       </c>
       <c r="H8">
-        <f>E8+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-19.279999999999994</v>
       </c>
       <c r="I8">
-        <f>$C$21+F8</f>
+        <f t="shared" si="1"/>
         <v>-18.479999999999997</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-19.18</v>
       </c>
       <c r="K8">
-        <f>$C$20*D8</f>
+        <f t="shared" si="2"/>
         <v>596.75815975503724</v>
       </c>
       <c r="L8">
-        <f>(1/$C$20)*C8</f>
+        <f t="shared" si="3"/>
         <v>320.4246089881571</v>
       </c>
       <c r="M8" s="1">
-        <f>D8*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>1.0419354838709676</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.0336277709295389</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8.3077129414286244E-3</v>
       </c>
       <c r="P8">
-        <f>(C8-$C$20*D8)^2</f>
+        <f t="shared" si="5"/>
         <v>22.640084254456056</v>
       </c>
     </row>
@@ -13370,39 +13370,39 @@
         <v>-66.900000000000006</v>
       </c>
       <c r="H9">
-        <f>E9+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-18.18</v>
       </c>
       <c r="I9">
-        <f>$C$21+F9</f>
+        <f t="shared" si="1"/>
         <v>-17.279999999999994</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-18.080000000000005</v>
       </c>
       <c r="K9">
-        <f>$C$20*D9</f>
+        <f t="shared" si="2"/>
         <v>731.62919895664004</v>
       </c>
       <c r="L9">
-        <f>(1/$C$20)*C9</f>
+        <f t="shared" si="3"/>
         <v>371.84409860618911</v>
       </c>
       <c r="M9" s="1">
-        <f>D9*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>1.2774193548387096</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.1994970922780293</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7.7922262560680355E-2</v>
       </c>
       <c r="P9">
-        <f>(C9-$C$20*D9)^2</f>
+        <f t="shared" si="5"/>
         <v>1991.7653995113603</v>
       </c>
     </row>
@@ -13426,35 +13426,35 @@
         <v>-66.3</v>
       </c>
       <c r="H10">
-        <f>E10+$C$21</f>
-        <v>-17.479999999999997</v>
-      </c>
-      <c r="I10">
-        <f>$C$21+F10</f>
-        <v>-16.68</v>
-      </c>
-      <c r="J10">
         <f t="shared" si="0"/>
         <v>-17.479999999999997</v>
       </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>-16.68</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>-17.479999999999997</v>
+      </c>
       <c r="K10">
-        <f>$C$20*D10</f>
+        <f t="shared" si="2"/>
         <v>812.92133217404455</v>
       </c>
       <c r="L10">
-        <f>(1/$C$20)*C10</f>
+        <f t="shared" si="3"/>
         <v>395.11818338066672</v>
       </c>
       <c r="M10" s="1">
-        <f>D10*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>1.4193548387096775</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.2745747850989246</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14478005361075286</v>
       </c>
     </row>
@@ -13478,35 +13478,35 @@
         <v>-65.8</v>
       </c>
       <c r="H11">
-        <f>E11+$C$21</f>
-        <v>-16.979999999999997</v>
-      </c>
-      <c r="I11">
-        <f>$C$21+F11</f>
-        <v>-16.279999999999994</v>
-      </c>
-      <c r="J11">
         <f t="shared" si="0"/>
         <v>-16.979999999999997</v>
       </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>-16.279999999999994</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>-16.979999999999997</v>
+      </c>
       <c r="K11">
-        <f>$C$20*D11</f>
+        <f t="shared" si="2"/>
         <v>875.73798056931162</v>
       </c>
       <c r="L11">
-        <f>(1/$C$20)*C11</f>
+        <f t="shared" si="3"/>
         <v>414.60346365697359</v>
       </c>
       <c r="M11" s="1">
-        <f>D11*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>1.5290322580645159</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.3374305279257213</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19160173013879467</v>
       </c>
     </row>
@@ -13530,35 +13530,35 @@
         <v>-64.7</v>
       </c>
       <c r="H12">
-        <f>E12+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-15.979999999999997</v>
       </c>
       <c r="I12">
-        <f>$C$21+F12</f>
+        <f t="shared" si="1"/>
         <v>-15.279999999999994</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-15.880000000000003</v>
       </c>
       <c r="K12">
-        <f>$C$20*D12</f>
+        <f t="shared" si="2"/>
         <v>1019.8467621819832</v>
       </c>
       <c r="L12">
-        <f>(1/$C$20)*C12</f>
+        <f t="shared" si="3"/>
         <v>444.9138996423398</v>
       </c>
       <c r="M12" s="1">
-        <f>D12*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>1.7806451612903225</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.4352061278785153</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.34543903341180715</v>
       </c>
     </row>
@@ -13582,35 +13582,35 @@
         <v>-63.8</v>
       </c>
       <c r="H13">
-        <f>E13+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-15.079999999999998</v>
       </c>
       <c r="I13">
-        <f>$C$21+F13</f>
+        <f t="shared" si="1"/>
         <v>-14.380000000000003</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-14.979999999999997</v>
       </c>
       <c r="K13">
-        <f>$C$20*D13</f>
+        <f t="shared" si="2"/>
         <v>1154.717801383586</v>
       </c>
       <c r="L13">
-        <f>(1/$C$20)*C13</f>
+        <f t="shared" si="3"/>
         <v>467.64672663136446</v>
       </c>
       <c r="M13" s="1">
-        <f>D13*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.0161290322580645</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5085378278431112</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.50759120441495331</v>
       </c>
     </row>
@@ -13634,35 +13634,35 @@
         <v>-63.1</v>
       </c>
       <c r="H14">
-        <f>E14+$C$21</f>
-        <v>-14.280000000000001</v>
-      </c>
-      <c r="I14">
-        <f>$C$21+F14</f>
-        <v>-13.479999999999997</v>
-      </c>
-      <c r="J14">
         <f t="shared" si="0"/>
         <v>-14.280000000000001</v>
       </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>-13.479999999999997</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>-14.280000000000001</v>
+      </c>
       <c r="K14">
-        <f>$C$20*D14</f>
+        <f t="shared" si="2"/>
         <v>1271.1133557630515</v>
       </c>
       <c r="L14">
-        <f>(1/$C$20)*C14</f>
+        <f t="shared" si="3"/>
         <v>478.4718823404238</v>
       </c>
       <c r="M14" s="1">
-        <f>D14*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.2193548387096773</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5434576849691088</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.67589715374056847</v>
       </c>
     </row>
@@ -13686,35 +13686,35 @@
         <v>-62.4</v>
       </c>
       <c r="H15">
-        <f>E15+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-13.479999999999997</v>
       </c>
       <c r="I15">
-        <f>$C$21+F15</f>
+        <f t="shared" si="1"/>
         <v>-12.780000000000001</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-13.579999999999998</v>
       </c>
       <c r="K15">
-        <f>$C$20*D15</f>
+        <f t="shared" si="2"/>
         <v>1365.3383283559522</v>
       </c>
       <c r="L15">
-        <f>(1/$C$20)*C15</f>
+        <f t="shared" si="3"/>
         <v>477.38936676951784</v>
       </c>
       <c r="M15" s="1">
-        <f>D15*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.3838709677419354</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5399656992565092</v>
       </c>
       <c r="O15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.84390526848542624</v>
       </c>
     </row>
@@ -13738,35 +13738,35 @@
         <v>-61.4</v>
       </c>
       <c r="H16">
-        <f>E16+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-12.780000000000001</v>
       </c>
       <c r="I16">
-        <f>$C$21+F16</f>
+        <f t="shared" si="1"/>
         <v>-12.280000000000001</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-12.579999999999998</v>
       </c>
       <c r="K16">
-        <f>$C$20*D16</f>
+        <f t="shared" si="2"/>
         <v>1448.4780100555702</v>
       </c>
       <c r="L16">
-        <f>(1/$C$20)*C16</f>
+        <f t="shared" si="3"/>
         <v>476.30685119861192</v>
       </c>
       <c r="M16" s="1">
-        <f>D16*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.5290322580645159</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5364737135439095</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.99255854452060643</v>
       </c>
     </row>
@@ -13790,35 +13790,35 @@
         <v>-60.7</v>
       </c>
       <c r="H17">
-        <f>E17+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-11.979999999999997</v>
       </c>
       <c r="I17">
-        <f>$C$21+F17</f>
+        <f t="shared" si="1"/>
         <v>-11.579999999999998</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-11.880000000000003</v>
       </c>
       <c r="K17">
-        <f>$C$20*D17</f>
+        <f t="shared" si="2"/>
         <v>1514.9897554152649</v>
       </c>
       <c r="L17">
-        <f>(1/$C$20)*C17</f>
+        <f t="shared" si="3"/>
         <v>476.30685119861192</v>
       </c>
       <c r="M17" s="1">
-        <f>D17*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.6451612903225805</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5364737135439095</v>
       </c>
       <c r="O17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.108687576778671</v>
       </c>
     </row>
@@ -13842,35 +13842,35 @@
         <v>-60</v>
       </c>
       <c r="H18">
-        <f>E18+$C$21</f>
+        <f t="shared" si="0"/>
         <v>-11.380000000000003</v>
       </c>
       <c r="I18">
-        <f>$C$21+F18</f>
+        <f t="shared" si="1"/>
         <v>-10.979999999999997</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>-11.18</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18" si="3">$C$20*D18</f>
+        <f t="shared" ref="K18" si="9">$C$20*D18</f>
         <v>1574.1113068461045</v>
       </c>
       <c r="L18">
-        <f>(1/$C$20)*C18</f>
+        <f t="shared" si="3"/>
         <v>476.30685119861192</v>
       </c>
       <c r="M18" s="1">
-        <f>D18*3.3/1023</f>
+        <f t="shared" si="4"/>
         <v>2.7483870967741932</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1.5364737135439095</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.2119133832302837</v>
       </c>
     </row>

</xml_diff>